<commit_message>
data cleaning , clock saving correctly files, CS correction
testing CS with weather years from more to less vres, and low CS value
</commit_message>
<xml_diff>
--- a/data/AMIRIS-EMLABpy Data inventoryREADME.xlsx
+++ b/data/AMIRIS-EMLABpy Data inventoryREADME.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCFD59E-0B08-4CD3-B4C6-B71E33DD7859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCA0C30-E307-4EE2-ABF7-4EC82BD6F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12315" yWindow="-16350" windowWidth="29040" windowHeight="15840" tabRatio="858" activeTab="1" xr2:uid="{06D6063F-292D-4EBB-8494-695710908624}"/>
+    <workbookView xWindow="28680" yWindow="-16515" windowWidth="29040" windowHeight="15840" tabRatio="858" xr2:uid="{06D6063F-292D-4EBB-8494-695710908624}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="6" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="40weatheryears" sheetId="9" r:id="rId3"/>
     <sheet name="Powerplants" sheetId="8" r:id="rId4"/>
     <sheet name="EMLABparameters" sheetId="1" r:id="rId5"/>
-    <sheet name="Exported_Traderes" sheetId="2" r:id="rId6"/>
+    <sheet name="Traderes_data" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="144">
   <si>
     <t>candidate power plants</t>
   </si>
@@ -369,9 +369,6 @@
     <t xml:space="preserve">technology and fuel prices </t>
   </si>
   <si>
-    <t>node</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -414,9 +411,6 @@
     <t>investmentCosts</t>
   </si>
   <si>
-    <t>unit2020, unit2030, unit2050</t>
-  </si>
-  <si>
     <t>2050 Static  load (households + non flexible inustrial) prepared from TNO</t>
   </si>
   <si>
@@ -450,12 +444,6 @@
     <t>TNO</t>
   </si>
   <si>
-    <t>check hydrogen and biomass</t>
-  </si>
-  <si>
-    <t>various (see excel)</t>
-  </si>
-  <si>
     <t>Fuels</t>
   </si>
   <si>
@@ -478,6 +466,15 @@
   </si>
   <si>
     <t xml:space="preserve">initial power plants </t>
+  </si>
+  <si>
+    <t>fuelprices</t>
+  </si>
+  <si>
+    <t>tech_specs</t>
+  </si>
+  <si>
+    <t>fixedcosts</t>
   </si>
 </sst>
 </file>
@@ -525,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -536,6 +533,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -553,10 +553,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -848,7 +844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -858,26 +854,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F790EBA3-A754-4E2E-8255-86BE883EA028}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="61.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="8" width="17.36328125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="1"/>
+    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -885,7 +881,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -905,7 +901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -925,7 +921,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -945,7 +941,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -962,7 +958,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -976,13 +972,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1002,7 +998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1022,12 +1018,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -1039,7 +1035,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1059,7 +1055,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1091,19 +1087,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEC486B-8D86-426D-B3C8-6DDE3231BED1}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.90625" customWidth="1"/>
-    <col min="3" max="3" width="57.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="61.81640625" customWidth="1"/>
-    <col min="5" max="5" width="45.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61.85546875" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1114,10 +1110,10 @@
         <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1125,16 +1121,16 @@
         <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1145,13 +1141,13 @@
         <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1162,7 +1158,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1186,15 +1182,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="76.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="22.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="76.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1205,7 +1201,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -1213,13 +1209,13 @@
         <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -1227,13 +1223,13 @@
         <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -1244,12 +1240,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>44</v>
@@ -1268,16 +1264,16 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="80.08984375" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="4" max="4" width="80.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1291,7 +1287,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1305,32 +1301,32 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>105</v>
       </c>
@@ -1344,21 +1340,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2ADC10-1ADB-4694-A77C-AC6F567EDBAF}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A8" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="2" max="2" width="33.7265625" customWidth="1"/>
-    <col min="3" max="3" width="33.90625" customWidth="1"/>
-    <col min="4" max="4" width="45.26953125" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" customWidth="1"/>
-    <col min="6" max="6" width="33.08984375" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1378,7 +1374,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1392,7 +1388,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>87</v>
       </c>
@@ -1400,12 +1396,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1416,10 +1412,10 @@
         <v>94</v>
       </c>
       <c r="F6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1430,10 +1426,10 @@
         <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1444,10 +1440,10 @@
         <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1458,15 +1454,15 @@
         <v>97</v>
       </c>
       <c r="F9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>6</v>
       </c>
@@ -1474,7 +1470,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>7</v>
       </c>
@@ -1482,7 +1478,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>8</v>
       </c>
@@ -1490,7 +1486,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>9</v>
       </c>
@@ -1498,12 +1494,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>11</v>
       </c>
@@ -1511,7 +1507,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>12</v>
       </c>
@@ -1519,7 +1515,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>13</v>
       </c>
@@ -1527,12 +1523,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>14</v>
       </c>
@@ -1543,7 +1539,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>61</v>
       </c>
@@ -1551,7 +1547,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>58</v>
       </c>
@@ -1559,7 +1555,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>68</v>
       </c>
@@ -1567,7 +1563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>16</v>
       </c>
@@ -1575,7 +1571,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>17</v>
       </c>
@@ -1583,7 +1579,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>69</v>
       </c>
@@ -1591,7 +1587,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>70</v>
       </c>
@@ -1599,7 +1595,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>71</v>
       </c>
@@ -1607,7 +1603,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>72</v>
       </c>
@@ -1618,7 +1614,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>73</v>
       </c>
@@ -1626,7 +1622,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>77</v>
       </c>
@@ -1637,7 +1633,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>15</v>
       </c>
@@ -1648,15 +1644,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>79</v>
       </c>
@@ -1664,7 +1660,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>80</v>
       </c>
@@ -1672,7 +1668,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>81</v>
       </c>
@@ -1680,7 +1676,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>82</v>
       </c>
@@ -1688,7 +1684,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>83</v>
       </c>
@@ -1696,7 +1692,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>84</v>
       </c>
@@ -1704,7 +1700,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>85</v>
       </c>
@@ -1712,7 +1708,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>2</v>
       </c>
@@ -1720,13 +1716,13 @@
         <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E43" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>89</v>
       </c>
@@ -1734,7 +1730,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>90</v>
       </c>
@@ -1742,7 +1738,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>91</v>
       </c>
@@ -1750,15 +1746,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E47" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1768,23 +1764,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519C8335-889B-4951-AA11-710FF5018BD1}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" customWidth="1"/>
-    <col min="3" max="3" width="29.36328125" customWidth="1"/>
-    <col min="4" max="4" width="42.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" customWidth="1"/>
-    <col min="6" max="6" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1801,122 +1797,128 @@
         <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>142</v>
+      </c>
       <c r="C6" t="s">
         <v>114</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="E6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>115</v>
       </c>
+      <c r="D7" s="6"/>
       <c r="E7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>116</v>
       </c>
+      <c r="D8" s="6"/>
       <c r="E8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>117</v>
       </c>
+      <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>118</v>
       </c>
+      <c r="D10" s="6"/>
       <c r="E10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>119</v>
       </c>
+      <c r="D11" s="6"/>
       <c r="E11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
         <v>120</v>
       </c>
-      <c r="E12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>108</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
+      <c r="E15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" t="s">
         <v>113</v>
       </c>
-      <c r="E15" t="s">
-        <v>121</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>135</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D6:D11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adapting workflow to increase demand according to excel input
</commit_message>
<xml_diff>
--- a/data/AMIRIS-EMLABpy Data inventoryREADME.xlsx
+++ b/data/AMIRIS-EMLABpy Data inventoryREADME.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCA0C30-E307-4EE2-ABF7-4EC82BD6F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C9842C-CD9B-4062-98D0-FA5281244D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-16515" windowWidth="29040" windowHeight="15840" tabRatio="858" xr2:uid="{06D6063F-292D-4EBB-8494-695710908624}"/>
+    <workbookView xWindow="-21810" yWindow="17250" windowWidth="29040" windowHeight="17640" tabRatio="858" activeTab="6" xr2:uid="{06D6063F-292D-4EBB-8494-695710908624}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="6" r:id="rId1"/>
@@ -19,8 +19,13 @@
     <sheet name="Powerplants" sheetId="8" r:id="rId4"/>
     <sheet name="EMLABparameters" sheetId="1" r:id="rId5"/>
     <sheet name="Traderes_data" sheetId="2" r:id="rId6"/>
+    <sheet name="CRM2050 paper" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="195">
   <si>
     <t>candidate power plants</t>
   </si>
@@ -475,13 +480,171 @@
   </si>
   <si>
     <t>fixedcosts</t>
+  </si>
+  <si>
+    <t>Biofuel</t>
+  </si>
+  <si>
+    <t>CCGT</t>
+  </si>
+  <si>
+    <t>CCS gas</t>
+  </si>
+  <si>
+    <t>Hard Coal</t>
+  </si>
+  <si>
+    <t>Hydro Reservoir</t>
+  </si>
+  <si>
+    <t>hydrogen CHP</t>
+  </si>
+  <si>
+    <t>hydrogen OCGT</t>
+  </si>
+  <si>
+    <t>hydrogen CCGT</t>
+  </si>
+  <si>
+    <t>Hydropower ROR</t>
+  </si>
+  <si>
+    <t>Lignite</t>
+  </si>
+  <si>
+    <t>Lithium ion battery</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>OCGT</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>PHS Discharge</t>
+  </si>
+  <si>
+    <t>Solar PV large</t>
+  </si>
+  <si>
+    <t>Solar PV rooftop</t>
+  </si>
+  <si>
+    <t>Wind Offshore</t>
+  </si>
+  <si>
+    <t>Wind Onshore</t>
+  </si>
+  <si>
+    <t>electrolyzer</t>
+  </si>
+  <si>
+    <t>central gas boiler</t>
+  </si>
+  <si>
+    <t>Lithium ion battery 4</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>nuclear</t>
+  </si>
+  <si>
+    <t>processing_residues</t>
+  </si>
+  <si>
+    <t>hydrogen</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>Eur/MWh</t>
+  </si>
+  <si>
+    <t>Technical lifetime</t>
+  </si>
+  <si>
+    <t>€/MW</t>
+  </si>
+  <si>
+    <t>node</t>
+  </si>
+  <si>
+    <t>CO2 (kg CO2/MWh)</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Fixed costs</t>
+  </si>
+  <si>
+    <t>Variable costs</t>
+  </si>
+  <si>
+    <t>Energy to Power Ratio</t>
+  </si>
+  <si>
+    <t>€/MWh</t>
+  </si>
+  <si>
+    <t>Technical limit</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>biofuel</t>
+  </si>
+  <si>
+    <t>Investment block</t>
+  </si>
+  <si>
+    <t>Max. lifetime extension</t>
+  </si>
+  <si>
+    <t>Permit time</t>
+  </si>
+  <si>
+    <t>Lead time</t>
+  </si>
+  <si>
+    <t>Investment costs</t>
+  </si>
+  <si>
+    <t>Charging efficiency</t>
+  </si>
+  <si>
+    <t>Discharging efficiency</t>
+  </si>
+  <si>
+    <t>Derating factor</t>
+  </si>
+  <si>
+    <t>Equity interest rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,8 +652,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,8 +704,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -518,11 +724,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -532,6 +770,49 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -539,8 +820,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{ECDBE5EE-B8EF-4258-BA78-D130336EB407}"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{9731BF3F-DEF8-4F32-922F-AA7C3667697A}"/>
+    <cellStyle name="Standard_Emission_factors" xfId="4" xr:uid="{395C6DAD-8EB4-4A1D-AADE-D709BBBCD4B6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -555,10 +840,1644 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="readme"/>
+      <sheetName val="DE"/>
+      <sheetName val="NL"/>
+      <sheetName val="investmentCosts"/>
+      <sheetName val="fixedCosts"/>
+      <sheetName val="fuelprices"/>
+      <sheetName val="lifetime_technical"/>
+      <sheetName val="techspecs"/>
+      <sheetName val="yearlyCO2"/>
+      <sheetName val="YearlyTargets"/>
+      <sheetName val="sources"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>traderesTechnology</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>MW</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Wind Onshore</v>
+          </cell>
+          <cell r="B2">
+            <v>12000</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Solar PV rooftop</v>
+          </cell>
+          <cell r="B3">
+            <v>26964</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Solar PV large</v>
+          </cell>
+          <cell r="B4">
+            <v>82099</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Wind Offshore</v>
+          </cell>
+          <cell r="B5">
+            <v>70000</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Biofuel</v>
+          </cell>
+          <cell r="B6">
+            <v>12040</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>OCGT</v>
+          </cell>
+          <cell r="B7">
+            <v>2700</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>technology</v>
+          </cell>
+          <cell r="B1">
+            <v>2050</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Biofuel</v>
+          </cell>
+          <cell r="B2">
+            <v>61676</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>CCGT</v>
+          </cell>
+          <cell r="B3">
+            <v>27647.69067</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>CCS gas</v>
+          </cell>
+          <cell r="B4">
+            <v>32000</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Hard Coal</v>
+          </cell>
+          <cell r="B5">
+            <v>61528.160000000003</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Hydro Reservoir</v>
+          </cell>
+          <cell r="B6">
+            <v>14207</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>hydrogen CHP</v>
+          </cell>
+          <cell r="B7">
+            <v>30000</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>hydrogen OCGT</v>
+          </cell>
+          <cell r="B8">
+            <v>7892.9478017180809</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>hydrogen CCGT</v>
+          </cell>
+          <cell r="B9">
+            <v>27647</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>Hydropower ROR</v>
+          </cell>
+          <cell r="B10">
+            <v>15715</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>Lignite</v>
+          </cell>
+          <cell r="B11">
+            <v>61528.160000000003</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>Lithium ion battery</v>
+          </cell>
+          <cell r="B12">
+            <v>570</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>Nuclear</v>
+          </cell>
+          <cell r="B13">
+            <v>111166.3</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>OCGT</v>
+          </cell>
+          <cell r="B14">
+            <v>7423</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="B15">
+            <v>8815.1</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>PHS Discharge</v>
+          </cell>
+          <cell r="B16">
+            <v>24222</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>Solar PV large</v>
+          </cell>
+          <cell r="B17">
+            <v>7400</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>Solar PV rooftop</v>
+          </cell>
+          <cell r="B18">
+            <v>8900</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Wind Offshore</v>
+          </cell>
+          <cell r="B19">
+            <v>33000</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Wind Onshore</v>
+          </cell>
+          <cell r="B20">
+            <v>12058.65</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>electrolyzer</v>
+          </cell>
+          <cell r="B21">
+            <v>28000.000000000004</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>central gas boiler</v>
+          </cell>
+          <cell r="B22">
+            <v>1700</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>Lithium ion battery 4</v>
+          </cell>
+          <cell r="B23">
+            <v>570</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Fuels keys</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>vom_cost</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>efficiency_full_load</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>ChargingEfficiency</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>EnergyToPowerRatio</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>DischargingEfficiency</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>lifetime_technical</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Biofuel</v>
+          </cell>
+          <cell r="B2">
+            <v>2.6</v>
+          </cell>
+          <cell r="C2">
+            <v>0.309</v>
+          </cell>
+          <cell r="D2">
+            <v>0</v>
+          </cell>
+          <cell r="E2">
+            <v>0</v>
+          </cell>
+          <cell r="F2">
+            <v>0</v>
+          </cell>
+          <cell r="G2">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>CCGT</v>
+          </cell>
+          <cell r="B3">
+            <v>4.4000000000000004</v>
+          </cell>
+          <cell r="C3">
+            <v>0.6</v>
+          </cell>
+          <cell r="D3">
+            <v>0</v>
+          </cell>
+          <cell r="E3">
+            <v>0</v>
+          </cell>
+          <cell r="F3">
+            <v>0</v>
+          </cell>
+          <cell r="G3">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>CCS gas</v>
+          </cell>
+          <cell r="B4">
+            <v>3</v>
+          </cell>
+          <cell r="C4">
+            <v>0.43</v>
+          </cell>
+          <cell r="D4">
+            <v>0</v>
+          </cell>
+          <cell r="E4">
+            <v>0</v>
+          </cell>
+          <cell r="F4">
+            <v>0</v>
+          </cell>
+          <cell r="G4">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Hard Coal</v>
+          </cell>
+          <cell r="B5">
+            <v>3.5</v>
+          </cell>
+          <cell r="C5">
+            <v>0.43</v>
+          </cell>
+          <cell r="D5">
+            <v>0</v>
+          </cell>
+          <cell r="E5">
+            <v>0</v>
+          </cell>
+          <cell r="F5">
+            <v>0</v>
+          </cell>
+          <cell r="G5">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Hydro Reservoir</v>
+          </cell>
+          <cell r="B6">
+            <v>1</v>
+          </cell>
+          <cell r="C6">
+            <v>1</v>
+          </cell>
+          <cell r="D6">
+            <v>0</v>
+          </cell>
+          <cell r="E6">
+            <v>0</v>
+          </cell>
+          <cell r="F6">
+            <v>0</v>
+          </cell>
+          <cell r="G6">
+            <v>60</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>hydrogen CHP</v>
+          </cell>
+          <cell r="B7">
+            <v>2.7</v>
+          </cell>
+          <cell r="C7">
+            <v>0.85</v>
+          </cell>
+          <cell r="D7">
+            <v>0</v>
+          </cell>
+          <cell r="E7">
+            <v>0</v>
+          </cell>
+          <cell r="F7">
+            <v>0</v>
+          </cell>
+          <cell r="G7">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>hydrogen OCGT</v>
+          </cell>
+          <cell r="B8">
+            <v>4.79</v>
+          </cell>
+          <cell r="C8">
+            <v>0.43</v>
+          </cell>
+          <cell r="D8">
+            <v>0</v>
+          </cell>
+          <cell r="E8">
+            <v>0</v>
+          </cell>
+          <cell r="F8">
+            <v>0</v>
+          </cell>
+          <cell r="G8">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>hydrogen CCGT</v>
+          </cell>
+          <cell r="B9">
+            <v>4.24</v>
+          </cell>
+          <cell r="C9">
+            <v>0.6</v>
+          </cell>
+          <cell r="D9">
+            <v>0</v>
+          </cell>
+          <cell r="E9">
+            <v>0</v>
+          </cell>
+          <cell r="F9">
+            <v>0</v>
+          </cell>
+          <cell r="G9">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>Hydropower ROR</v>
+          </cell>
+          <cell r="B10">
+            <v>0</v>
+          </cell>
+          <cell r="C10">
+            <v>1</v>
+          </cell>
+          <cell r="D10">
+            <v>0</v>
+          </cell>
+          <cell r="E10">
+            <v>0</v>
+          </cell>
+          <cell r="F10">
+            <v>0</v>
+          </cell>
+          <cell r="G10">
+            <v>60</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>Lignite</v>
+          </cell>
+          <cell r="B11">
+            <v>3.5</v>
+          </cell>
+          <cell r="C11">
+            <v>0.43</v>
+          </cell>
+          <cell r="D11">
+            <v>0</v>
+          </cell>
+          <cell r="E11">
+            <v>0</v>
+          </cell>
+          <cell r="F11">
+            <v>0</v>
+          </cell>
+          <cell r="G11">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>Lithium ion battery</v>
+          </cell>
+          <cell r="B12">
+            <v>1.8</v>
+          </cell>
+          <cell r="C12">
+            <v>0.92</v>
+          </cell>
+          <cell r="D12">
+            <v>0.92</v>
+          </cell>
+          <cell r="E12">
+            <v>2</v>
+          </cell>
+          <cell r="F12">
+            <v>0.92</v>
+          </cell>
+          <cell r="G12">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>Nuclear</v>
+          </cell>
+          <cell r="B13">
+            <v>3.5</v>
+          </cell>
+          <cell r="C13">
+            <v>0.35</v>
+          </cell>
+          <cell r="D13">
+            <v>0</v>
+          </cell>
+          <cell r="E13">
+            <v>0</v>
+          </cell>
+          <cell r="F13">
+            <v>0</v>
+          </cell>
+          <cell r="G13">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>OCGT</v>
+          </cell>
+          <cell r="B14">
+            <v>4.5</v>
+          </cell>
+          <cell r="C14">
+            <v>0.43</v>
+          </cell>
+          <cell r="D14">
+            <v>0</v>
+          </cell>
+          <cell r="E14">
+            <v>0</v>
+          </cell>
+          <cell r="F14">
+            <v>0</v>
+          </cell>
+          <cell r="G14">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="B15">
+            <v>3.5</v>
+          </cell>
+          <cell r="C15">
+            <v>0.43</v>
+          </cell>
+          <cell r="D15">
+            <v>0</v>
+          </cell>
+          <cell r="E15">
+            <v>0</v>
+          </cell>
+          <cell r="F15">
+            <v>0</v>
+          </cell>
+          <cell r="G15">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>PHS Discharge</v>
+          </cell>
+          <cell r="B16">
+            <v>1</v>
+          </cell>
+          <cell r="C16">
+            <v>1</v>
+          </cell>
+          <cell r="D16">
+            <v>0.89</v>
+          </cell>
+          <cell r="E16">
+            <v>10</v>
+          </cell>
+          <cell r="F16">
+            <v>0.89</v>
+          </cell>
+          <cell r="G16">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>Solar PV large</v>
+          </cell>
+          <cell r="B17">
+            <v>0.5</v>
+          </cell>
+          <cell r="C17">
+            <v>1</v>
+          </cell>
+          <cell r="D17">
+            <v>0</v>
+          </cell>
+          <cell r="E17">
+            <v>0</v>
+          </cell>
+          <cell r="F17">
+            <v>0</v>
+          </cell>
+          <cell r="G17">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>Solar PV rooftop</v>
+          </cell>
+          <cell r="B18">
+            <v>0.5</v>
+          </cell>
+          <cell r="C18">
+            <v>1</v>
+          </cell>
+          <cell r="D18">
+            <v>0</v>
+          </cell>
+          <cell r="E18">
+            <v>0</v>
+          </cell>
+          <cell r="F18">
+            <v>0</v>
+          </cell>
+          <cell r="G18">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Wind Offshore</v>
+          </cell>
+          <cell r="B19">
+            <v>0.5</v>
+          </cell>
+          <cell r="C19">
+            <v>1</v>
+          </cell>
+          <cell r="D19">
+            <v>0</v>
+          </cell>
+          <cell r="E19">
+            <v>0</v>
+          </cell>
+          <cell r="F19">
+            <v>0</v>
+          </cell>
+          <cell r="G19">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Wind Onshore</v>
+          </cell>
+          <cell r="B20">
+            <v>2</v>
+          </cell>
+          <cell r="C20">
+            <v>1</v>
+          </cell>
+          <cell r="D20">
+            <v>0</v>
+          </cell>
+          <cell r="E20">
+            <v>0</v>
+          </cell>
+          <cell r="F20">
+            <v>0</v>
+          </cell>
+          <cell r="G20">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>electrolyzer</v>
+          </cell>
+          <cell r="B21">
+            <v>0</v>
+          </cell>
+          <cell r="C21">
+            <v>0.74</v>
+          </cell>
+          <cell r="D21">
+            <v>0</v>
+          </cell>
+          <cell r="E21">
+            <v>0</v>
+          </cell>
+          <cell r="F21">
+            <v>0</v>
+          </cell>
+          <cell r="G21">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>central gas boiler</v>
+          </cell>
+          <cell r="B22">
+            <v>1</v>
+          </cell>
+          <cell r="C22">
+            <v>1.04</v>
+          </cell>
+          <cell r="D22">
+            <v>0</v>
+          </cell>
+          <cell r="E22">
+            <v>0</v>
+          </cell>
+          <cell r="F22">
+            <v>0</v>
+          </cell>
+          <cell r="G22">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>Lithium ion battery 4</v>
+          </cell>
+          <cell r="B23">
+            <v>1.8</v>
+          </cell>
+          <cell r="C23">
+            <v>0.92</v>
+          </cell>
+          <cell r="D23">
+            <v>0.92</v>
+          </cell>
+          <cell r="E23">
+            <v>4</v>
+          </cell>
+          <cell r="F23">
+            <v>0.92</v>
+          </cell>
+          <cell r="G23">
+            <v>25</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="explanation"/>
+      <sheetName val="dictTech"/>
+      <sheetName val="dictFuel"/>
+      <sheetName val="TechnologyTargets"/>
+      <sheetName val="CapacityMarkets"/>
+      <sheetName val="StrategicReserveOperator"/>
+      <sheetName val="ElectricitySpotMarkets"/>
+      <sheetName val="peakLoad"/>
+      <sheetName val="Fuels"/>
+      <sheetName val="FuelPriceTrends"/>
+      <sheetName val="CandidatePowerPlants"/>
+      <sheetName val="TechnologiesEmlab"/>
+      <sheetName val="derating"/>
+      <sheetName val="TechnologyTrends"/>
+      <sheetName val="EnergyProducers"/>
+      <sheetName val="LoadShifterCap"/>
+      <sheetName val="CapacitySubscriptionConsumer"/>
+      <sheetName val="CS_subscribed"/>
+      <sheetName val="LoadShedders"/>
+      <sheetName val="LSyearly"/>
+      <sheetName val="Dismantled"/>
+      <sheetName val="weatherYears40"/>
+      <sheetName val="VOLLs"/>
+      <sheetName val="LoadShedders_feb24"/>
+      <sheetName val="LoadShedders (2)"/>
+      <sheetName val="LoadShedders2"/>
+      <sheetName val="LoadShedders_copy"/>
+      <sheetName val="dictvariables"/>
+      <sheetName val="StepTrends"/>
+      <sheetName val="EnergyConsumers"/>
+      <sheetName val="yearlytechnologyPotentials2"/>
+      <sheetName val="graphs"/>
+      <sheetName val="CO2DE"/>
+      <sheetName val="backup"/>
+      <sheetName val="weatherYearsOLD"/>
+      <sheetName val="sources"/>
+      <sheetName val="NewTechnologies"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Technology</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>ViableInvestment</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Realistic_capacity</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Lithium ion battery</v>
+          </cell>
+          <cell r="C2" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="D2">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Wind Offshore</v>
+          </cell>
+          <cell r="C3" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="D3">
+            <v>500</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>hydrogen CCGT</v>
+          </cell>
+          <cell r="C4" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="D4">
+            <v>400</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Solar PV large</v>
+          </cell>
+          <cell r="C5" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="D5">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>Wind Onshore</v>
+          </cell>
+          <cell r="C6" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="D6">
+            <v>500</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Biofuel</v>
+          </cell>
+          <cell r="C7" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="D7">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>hydrogen OCGT</v>
+          </cell>
+          <cell r="C8" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="D8">
+            <v>400</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Lithium ion battery 4</v>
+          </cell>
+          <cell r="C9" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="D9">
+            <v>300</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>traderes technology</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>type</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>expectedPermittime</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>expectedLeadtime</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Intermittent</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>MaximumLifeExtension</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>deratingFactor</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>traderesfuels</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>interest_rate</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>hydrogen OCGT</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C2">
+            <v>2</v>
+          </cell>
+          <cell r="D2">
+            <v>2</v>
+          </cell>
+          <cell r="E2" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F2">
+            <v>6</v>
+          </cell>
+          <cell r="G2">
+            <v>1</v>
+          </cell>
+          <cell r="H2" t="str">
+            <v>hydrogen</v>
+          </cell>
+          <cell r="I2">
+            <v>0.08</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>hydrogen CCGT</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C3">
+            <v>2</v>
+          </cell>
+          <cell r="D3">
+            <v>2</v>
+          </cell>
+          <cell r="E3" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F3">
+            <v>6</v>
+          </cell>
+          <cell r="G3">
+            <v>1</v>
+          </cell>
+          <cell r="H3" t="str">
+            <v>hydrogen</v>
+          </cell>
+          <cell r="I3">
+            <v>0.08</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Biofuel</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C4">
+            <v>1</v>
+          </cell>
+          <cell r="D4">
+            <v>3</v>
+          </cell>
+          <cell r="E4" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F4">
+            <v>6</v>
+          </cell>
+          <cell r="G4">
+            <v>1</v>
+          </cell>
+          <cell r="H4" t="str">
+            <v>biomethane</v>
+          </cell>
+          <cell r="I4">
+            <v>0.05</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Lithium ion battery 4</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>StorageTrader</v>
+          </cell>
+          <cell r="C5">
+            <v>0</v>
+          </cell>
+          <cell r="D5">
+            <v>1</v>
+          </cell>
+          <cell r="E5" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F5">
+            <v>1</v>
+          </cell>
+          <cell r="G5">
+            <v>0.25</v>
+          </cell>
+          <cell r="I5">
+            <v>0.05</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Lithium ion battery</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>StorageTrader</v>
+          </cell>
+          <cell r="C6">
+            <v>0</v>
+          </cell>
+          <cell r="D6">
+            <v>1</v>
+          </cell>
+          <cell r="E6" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F6">
+            <v>1</v>
+          </cell>
+          <cell r="G6">
+            <v>0.16</v>
+          </cell>
+          <cell r="I6">
+            <v>0.05</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>Nuclear</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C7">
+            <v>2</v>
+          </cell>
+          <cell r="D7">
+            <v>5</v>
+          </cell>
+          <cell r="E7" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F7">
+            <v>20</v>
+          </cell>
+          <cell r="G7">
+            <v>1</v>
+          </cell>
+          <cell r="H7" t="str">
+            <v>nuclear</v>
+          </cell>
+          <cell r="I7">
+            <v>0.08</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>Solar PV large</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>VariableRenewableOperator</v>
+          </cell>
+          <cell r="C8">
+            <v>1</v>
+          </cell>
+          <cell r="D8">
+            <v>1</v>
+          </cell>
+          <cell r="E8" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="F8">
+            <v>3</v>
+          </cell>
+          <cell r="G8">
+            <v>0</v>
+          </cell>
+          <cell r="I8">
+            <v>0.05</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>Solar PV rooftop</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>VariableRenewableOperator</v>
+          </cell>
+          <cell r="C9">
+            <v>1</v>
+          </cell>
+          <cell r="D9">
+            <v>1</v>
+          </cell>
+          <cell r="E9" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="F9">
+            <v>3</v>
+          </cell>
+          <cell r="G9">
+            <v>0</v>
+          </cell>
+          <cell r="I9">
+            <v>0.05</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>Wind Offshore</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>VariableRenewableOperator</v>
+          </cell>
+          <cell r="C10">
+            <v>1</v>
+          </cell>
+          <cell r="D10">
+            <v>2</v>
+          </cell>
+          <cell r="E10" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="F10">
+            <v>5</v>
+          </cell>
+          <cell r="G10">
+            <v>0.06</v>
+          </cell>
+          <cell r="I10">
+            <v>0.05</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>Wind Onshore</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>VariableRenewableOperator</v>
+          </cell>
+          <cell r="C11">
+            <v>1</v>
+          </cell>
+          <cell r="D11">
+            <v>2</v>
+          </cell>
+          <cell r="E11" t="b">
+            <v>1</v>
+          </cell>
+          <cell r="F11">
+            <v>4</v>
+          </cell>
+          <cell r="G11">
+            <v>0.12</v>
+          </cell>
+          <cell r="I11">
+            <v>0.05</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>electrolyzer</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C12">
+            <v>0</v>
+          </cell>
+          <cell r="D12">
+            <v>0</v>
+          </cell>
+          <cell r="E12" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F12">
+            <v>0</v>
+          </cell>
+          <cell r="G12">
+            <v>0</v>
+          </cell>
+          <cell r="I12">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>central gas boiler</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C13">
+            <v>0</v>
+          </cell>
+          <cell r="D13">
+            <v>0</v>
+          </cell>
+          <cell r="E13" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F13">
+            <v>0</v>
+          </cell>
+          <cell r="G13">
+            <v>1</v>
+          </cell>
+          <cell r="H13" t="str">
+            <v>natural_gas</v>
+          </cell>
+          <cell r="I13">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>CCGT</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C14">
+            <v>1</v>
+          </cell>
+          <cell r="D14">
+            <v>2</v>
+          </cell>
+          <cell r="E14" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F14">
+            <v>5</v>
+          </cell>
+          <cell r="G14">
+            <v>1</v>
+          </cell>
+          <cell r="H14" t="str">
+            <v>natural_gas</v>
+          </cell>
+          <cell r="I14">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>CCS gas</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C15">
+            <v>1</v>
+          </cell>
+          <cell r="D15">
+            <v>2</v>
+          </cell>
+          <cell r="E15" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F15">
+            <v>5</v>
+          </cell>
+          <cell r="G15">
+            <v>1</v>
+          </cell>
+          <cell r="H15" t="str">
+            <v>natural_gas</v>
+          </cell>
+          <cell r="I15">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>Hard Coal</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C16">
+            <v>1</v>
+          </cell>
+          <cell r="D16">
+            <v>4</v>
+          </cell>
+          <cell r="E16" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F16">
+            <v>10</v>
+          </cell>
+          <cell r="G16">
+            <v>1</v>
+          </cell>
+          <cell r="H16" t="str">
+            <v>hard_coal</v>
+          </cell>
+          <cell r="I16">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>Hydro Reservoir</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>VariableRenewableOperator</v>
+          </cell>
+          <cell r="C17">
+            <v>5</v>
+          </cell>
+          <cell r="D17">
+            <v>5</v>
+          </cell>
+          <cell r="E17" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F17">
+            <v>20</v>
+          </cell>
+          <cell r="G17">
+            <v>0.9</v>
+          </cell>
+          <cell r="I17">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>hydrogen CHP</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C18">
+            <v>2</v>
+          </cell>
+          <cell r="D18">
+            <v>2</v>
+          </cell>
+          <cell r="E18" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F18">
+            <v>5</v>
+          </cell>
+          <cell r="G18">
+            <v>1</v>
+          </cell>
+          <cell r="H18" t="str">
+            <v>hydrogen</v>
+          </cell>
+          <cell r="I18">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Hydropower ROR</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>VariableRenewableOperator</v>
+          </cell>
+          <cell r="C19">
+            <v>5</v>
+          </cell>
+          <cell r="D19">
+            <v>5</v>
+          </cell>
+          <cell r="E19" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F19">
+            <v>20</v>
+          </cell>
+          <cell r="G19">
+            <v>0.41</v>
+          </cell>
+          <cell r="I19">
+            <v>0.05</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Lignite</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C20">
+            <v>1</v>
+          </cell>
+          <cell r="D20">
+            <v>5</v>
+          </cell>
+          <cell r="E20" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F20">
+            <v>5</v>
+          </cell>
+          <cell r="G20">
+            <v>1</v>
+          </cell>
+          <cell r="H20" t="str">
+            <v>lignite</v>
+          </cell>
+          <cell r="I20">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>OCGT</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C21">
+            <v>1</v>
+          </cell>
+          <cell r="D21">
+            <v>2</v>
+          </cell>
+          <cell r="E21" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F21">
+            <v>5</v>
+          </cell>
+          <cell r="G21">
+            <v>1</v>
+          </cell>
+          <cell r="H21" t="str">
+            <v>natural_gas</v>
+          </cell>
+          <cell r="I21">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>ConventionalPlantOperator</v>
+          </cell>
+          <cell r="C22">
+            <v>1</v>
+          </cell>
+          <cell r="D22">
+            <v>1</v>
+          </cell>
+          <cell r="E22" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F22">
+            <v>5</v>
+          </cell>
+          <cell r="G22">
+            <v>1</v>
+          </cell>
+          <cell r="H22" t="str">
+            <v>oil</v>
+          </cell>
+          <cell r="I22">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>PHS Discharge</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>StorageTrader</v>
+          </cell>
+          <cell r="C23">
+            <v>3</v>
+          </cell>
+          <cell r="D23">
+            <v>4</v>
+          </cell>
+          <cell r="E23" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="F23">
+            <v>20</v>
+          </cell>
+          <cell r="G23">
+            <v>0.9</v>
+          </cell>
+          <cell r="I23">
+            <v>0.05</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -596,7 +2515,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -702,7 +2621,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -844,7 +2763,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -854,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F790EBA3-A754-4E2E-8255-86BE883EA028}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,14 +2791,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1340,7 +3259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2ADC10-1ADB-4694-A77C-AC6F567EDBAF}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1767,7 +3686,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,7 +3753,7 @@
       <c r="C6" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="33" t="s">
         <v>131</v>
       </c>
       <c r="E6" t="s">
@@ -1845,7 +3764,7 @@
       <c r="C7" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="33"/>
       <c r="E7" t="s">
         <v>120</v>
       </c>
@@ -1854,7 +3773,7 @@
       <c r="C8" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="33"/>
       <c r="E8" t="s">
         <v>120</v>
       </c>
@@ -1863,7 +3782,7 @@
       <c r="C9" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="33"/>
       <c r="E9" t="s">
         <v>120</v>
       </c>
@@ -1872,7 +3791,7 @@
       <c r="C10" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="33"/>
       <c r="E10" t="s">
         <v>120</v>
       </c>
@@ -1881,7 +3800,7 @@
       <c r="C11" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="33"/>
       <c r="E11" t="s">
         <v>120</v>
       </c>
@@ -1921,4 +3840,1396 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7687DA7-3C2C-45D0-9AF0-6FFA33519AD9}">
+  <dimension ref="A1:R54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2400000</v>
+      </c>
+      <c r="C3" s="17">
+        <f>VLOOKUP(A3,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>61676</v>
+      </c>
+      <c r="D3" s="20">
+        <f>VLOOKUP($A3,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>2.6</v>
+      </c>
+      <c r="E3" s="17">
+        <f>R3*100</f>
+        <v>30.9</v>
+      </c>
+      <c r="F3" s="20">
+        <f>VLOOKUP($A3,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="20">
+        <f>VLOOKUP($A3,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="20">
+        <f>VLOOKUP($A3,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="17">
+        <f>VLOOKUP($A3,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+      <c r="J3" s="17">
+        <f>VLOOKUP(A3,[1]NL!$A$1:$B$7,2,0)</f>
+        <v>12040</v>
+      </c>
+      <c r="R3" s="20">
+        <f>VLOOKUP($A3,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="17">
+        <v>435982.81438000005</v>
+      </c>
+      <c r="C4" s="17">
+        <f>VLOOKUP(A4,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>7892.9478017180809</v>
+      </c>
+      <c r="D4" s="20">
+        <f>VLOOKUP($A4,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>4.79</v>
+      </c>
+      <c r="E4" s="17">
+        <f>R4*100</f>
+        <v>43</v>
+      </c>
+      <c r="F4" s="20">
+        <f>VLOOKUP($A4,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="20">
+        <f>VLOOKUP($A4,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="20">
+        <f>VLOOKUP($A4,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="17">
+        <f>VLOOKUP($A4,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="20">
+        <f>VLOOKUP($A4,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="17">
+        <v>850698.174</v>
+      </c>
+      <c r="C5" s="17">
+        <f>VLOOKUP(A5,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>27647</v>
+      </c>
+      <c r="D5" s="20">
+        <f>VLOOKUP($A5,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>4.24</v>
+      </c>
+      <c r="E5" s="17">
+        <f>R5*100</f>
+        <v>60</v>
+      </c>
+      <c r="F5" s="20">
+        <f>VLOOKUP($A5,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="20">
+        <f>VLOOKUP($A5,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
+        <f>VLOOKUP($A5,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="17">
+        <f>VLOOKUP($A5,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" s="20">
+        <f>VLOOKUP($A5,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="17">
+        <v>220000</v>
+      </c>
+      <c r="C6" s="17">
+        <f>VLOOKUP(A6,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>570</v>
+      </c>
+      <c r="D6" s="20">
+        <f>VLOOKUP($A6,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>1.8</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="17">
+        <f>VLOOKUP($A6,[1]techspecs!$A$1:$G$23,4,0)*100</f>
+        <v>92</v>
+      </c>
+      <c r="G6" s="17">
+        <f>VLOOKUP($A6,[1]techspecs!$A$1:$G$23,6,0)*100</f>
+        <v>92</v>
+      </c>
+      <c r="H6" s="17">
+        <f>VLOOKUP($A6,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="17">
+        <f>VLOOKUP($A6,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" s="20">
+        <f>VLOOKUP($A6,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="17">
+        <v>380000</v>
+      </c>
+      <c r="C7" s="17">
+        <f>VLOOKUP(A7,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>570</v>
+      </c>
+      <c r="D7" s="20">
+        <f>VLOOKUP($A7,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>1.8</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="17">
+        <f>VLOOKUP($A7,[1]techspecs!$A$1:$G$23,4,0)*100</f>
+        <v>92</v>
+      </c>
+      <c r="G7" s="17">
+        <f>VLOOKUP($A7,[1]techspecs!$A$1:$G$23,6,0)*100</f>
+        <v>92</v>
+      </c>
+      <c r="H7" s="17">
+        <f>VLOOKUP($A7,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>4</v>
+      </c>
+      <c r="I7" s="17">
+        <f>VLOOKUP($A7,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="R7" s="20">
+        <f>VLOOKUP($A7,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="17">
+        <v>7940450</v>
+      </c>
+      <c r="C8" s="17">
+        <f>VLOOKUP(A8,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>111166.3</v>
+      </c>
+      <c r="D8" s="20">
+        <f>VLOOKUP($A8,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="17">
+        <f>R8*100</f>
+        <v>35</v>
+      </c>
+      <c r="F8" s="20">
+        <f>VLOOKUP($A8,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="20">
+        <f>VLOOKUP($A8,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="20">
+        <f>VLOOKUP($A8,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="17">
+        <f>VLOOKUP($A8,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>40</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="R8" s="20">
+        <f>VLOOKUP($A8,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="17">
+        <v>290000</v>
+      </c>
+      <c r="C9" s="17">
+        <f>VLOOKUP(A9,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>7400</v>
+      </c>
+      <c r="D9" s="20">
+        <f>VLOOKUP($A9,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="20">
+        <f>VLOOKUP($A9,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="20">
+        <f>VLOOKUP($A9,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="20">
+        <f>VLOOKUP($A9,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="20">
+        <f>VLOOKUP($A9,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
+        <f>VLOOKUP($A9,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+      <c r="J9" s="17">
+        <f>VLOOKUP(A9,[1]NL!$A$1:$B$7,2,0)</f>
+        <v>82099</v>
+      </c>
+      <c r="R9" s="20">
+        <f>VLOOKUP($A9,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="17">
+        <v>640000</v>
+      </c>
+      <c r="C10" s="17">
+        <f>VLOOKUP(A10,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>8900</v>
+      </c>
+      <c r="D10" s="20">
+        <f>VLOOKUP($A10,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="20">
+        <f>VLOOKUP($A10,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="20">
+        <f>VLOOKUP($A10,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="20">
+        <f>VLOOKUP($A10,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="20">
+        <f>VLOOKUP($A10,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <f>VLOOKUP($A10,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+      <c r="J10" s="17">
+        <f>VLOOKUP(A10,[1]NL!$A$1:$B$7,2,0)</f>
+        <v>26964</v>
+      </c>
+      <c r="R10" s="20">
+        <f>VLOOKUP($A10,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1640000</v>
+      </c>
+      <c r="C11" s="17">
+        <f>VLOOKUP(A11,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>33000</v>
+      </c>
+      <c r="D11" s="20">
+        <f>VLOOKUP($A11,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="20">
+        <f>VLOOKUP($A11,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="20">
+        <f>VLOOKUP($A11,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="20">
+        <f>VLOOKUP($A11,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="20">
+        <f>VLOOKUP($A11,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <f>VLOOKUP($A11,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>30</v>
+      </c>
+      <c r="J11" s="17">
+        <f>VLOOKUP(A11,[1]NL!$A$1:$B$7,2,0)</f>
+        <v>70000</v>
+      </c>
+      <c r="R11" s="20">
+        <f>VLOOKUP($A11,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="17">
+        <v>1090288.1746699999</v>
+      </c>
+      <c r="C12" s="17">
+        <f>VLOOKUP(A12,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>12058.65</v>
+      </c>
+      <c r="D12" s="20">
+        <f>VLOOKUP($A12,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="20">
+        <f>VLOOKUP($A12,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="20">
+        <f>VLOOKUP($A12,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="20">
+        <f>VLOOKUP($A12,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="20">
+        <f>VLOOKUP($A12,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="17">
+        <f>VLOOKUP($A12,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>30</v>
+      </c>
+      <c r="J12" s="17">
+        <f>VLOOKUP(A12,[1]NL!$A$1:$B$7,2,0)</f>
+        <v>12000</v>
+      </c>
+      <c r="R12" s="20">
+        <f>VLOOKUP($A12,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="K13" s="27"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="R13" s="30"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="H14" s="30"/>
+      <c r="I14" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="K14" s="27"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="R14" s="30"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="16">
+        <f>VLOOKUP(A3,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C15" s="16">
+        <f>VLOOKUP(A3,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="16">
+        <f>VLOOKUP(A3,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>3</v>
+      </c>
+      <c r="E15" s="16">
+        <f>VLOOKUP(A3,[2]CandidatePowerPlants!$B$1:$D$9,3,0)</f>
+        <v>300</v>
+      </c>
+      <c r="F15" s="29">
+        <f>VLOOKUP(A3,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>5</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="29">
+        <f>VLOOKUP(A3,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>100</v>
+      </c>
+      <c r="K15" s="27"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="R15" s="30"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="16">
+        <f>VLOOKUP(A4,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C16" s="16">
+        <f>VLOOKUP(A4,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D16" s="16">
+        <f>VLOOKUP(A4,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E16" s="16">
+        <f>VLOOKUP(A4,[2]CandidatePowerPlants!$B$1:$D$9,3,0)</f>
+        <v>400</v>
+      </c>
+      <c r="F16" s="29">
+        <f>VLOOKUP(A4,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>8</v>
+      </c>
+      <c r="H16" s="30"/>
+      <c r="I16" s="29">
+        <f>VLOOKUP(A4,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>100</v>
+      </c>
+      <c r="K16" s="27"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="R16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="16">
+        <f>VLOOKUP(A5,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C17" s="16">
+        <f>VLOOKUP(A5,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D17" s="16">
+        <f>VLOOKUP(A5,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E17" s="16">
+        <f>VLOOKUP(A5,[2]CandidatePowerPlants!$B$1:$D$9,3,0)</f>
+        <v>400</v>
+      </c>
+      <c r="F17" s="29">
+        <f>VLOOKUP(A5,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>8</v>
+      </c>
+      <c r="I17" s="29">
+        <f>VLOOKUP(A5,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="16">
+        <f>VLOOKUP(A6,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="16">
+        <f>VLOOKUP(A6,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="16">
+        <f>VLOOKUP(A6,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <f>VLOOKUP(A6,[2]CandidatePowerPlants!$B$1:$D$9,3,0)</f>
+        <v>300</v>
+      </c>
+      <c r="F18" s="29">
+        <f>VLOOKUP(A6,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>5</v>
+      </c>
+      <c r="I18" s="29">
+        <f>VLOOKUP(A6,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="16">
+        <f>VLOOKUP(A7,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="16">
+        <f>VLOOKUP(A7,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="16">
+        <f>VLOOKUP(A7,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="16">
+        <f>VLOOKUP(A7,[2]CandidatePowerPlants!$B$1:$D$9,3,0)</f>
+        <v>300</v>
+      </c>
+      <c r="F19" s="29">
+        <f>VLOOKUP(A7,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>5</v>
+      </c>
+      <c r="I19" s="29">
+        <f>VLOOKUP(A7,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="16">
+        <f>VLOOKUP(A8,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>20</v>
+      </c>
+      <c r="C20" s="16">
+        <f>VLOOKUP(A8,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D20" s="16">
+        <f>VLOOKUP(A8,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>5</v>
+      </c>
+      <c r="E20" s="16">
+        <v>1000</v>
+      </c>
+      <c r="F20" s="29">
+        <f>VLOOKUP(A8,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>8</v>
+      </c>
+      <c r="I20" s="29">
+        <f>VLOOKUP(A8,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="16">
+        <f>VLOOKUP(A9,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C21" s="16">
+        <f>VLOOKUP(A9,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="16">
+        <f>VLOOKUP(A9,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="16">
+        <f>VLOOKUP(A9,[2]CandidatePowerPlants!$B$1:$D$9,3,0)</f>
+        <v>300</v>
+      </c>
+      <c r="F21" s="29">
+        <f>VLOOKUP(A9,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>5</v>
+      </c>
+      <c r="I21" s="29">
+        <f>VLOOKUP(A9,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="16">
+        <f>VLOOKUP(A10,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C22" s="16">
+        <f>VLOOKUP(A10,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="16">
+        <f>VLOOKUP(A10,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E22" s="16">
+        <v>300</v>
+      </c>
+      <c r="F22" s="29">
+        <f>VLOOKUP(A10,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>5</v>
+      </c>
+      <c r="I22" s="29">
+        <f>VLOOKUP(A10,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="16">
+        <f>VLOOKUP(A11,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>5</v>
+      </c>
+      <c r="C23" s="16">
+        <f>VLOOKUP(A11,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="16">
+        <f>VLOOKUP(A11,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E23" s="16">
+        <f>VLOOKUP(A11,[2]CandidatePowerPlants!$B$1:$D$9,3,0)</f>
+        <v>500</v>
+      </c>
+      <c r="F23" s="29">
+        <f>VLOOKUP(A11,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>5</v>
+      </c>
+      <c r="I23" s="29">
+        <f>VLOOKUP(A11,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B24" s="16">
+        <f>VLOOKUP(A12,[2]TechnologiesEmlab!$A$1:$I$24,6,0)</f>
+        <v>4</v>
+      </c>
+      <c r="C24" s="16">
+        <f>VLOOKUP(A12,[2]TechnologiesEmlab!$A$1:$I$23,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="16">
+        <f>VLOOKUP(A12,[2]TechnologiesEmlab!$A$1:$I$23,4,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E24" s="16">
+        <f>VLOOKUP(A12,[2]CandidatePowerPlants!$B$1:$D$9,3,0)</f>
+        <v>500</v>
+      </c>
+      <c r="F24" s="29">
+        <f>VLOOKUP(A12,[2]TechnologiesEmlab!$A$1:$I$23,9,0)*100</f>
+        <v>5</v>
+      </c>
+      <c r="I24" s="29">
+        <f>VLOOKUP(A12,[2]TechnologiesEmlab!$A$1:$I$23,7,0)*100</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" s="7">
+        <f>ROUND(2970000*1.002*1.016*1.018*1.014*1.007,0)</f>
+        <v>3142918</v>
+      </c>
+      <c r="C27" s="11">
+        <f>VLOOKUP(A27,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>15715</v>
+      </c>
+      <c r="D27">
+        <f>VLOOKUP($A27,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>VLOOKUP($A27,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f>VLOOKUP($A27,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>VLOOKUP($A27,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f>VLOOKUP($A27,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f>VLOOKUP($A27,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="11">
+        <f>VLOOKUP(A28,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>61528.160000000003</v>
+      </c>
+      <c r="D28">
+        <f>VLOOKUP($A28,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>3.5</v>
+      </c>
+      <c r="E28">
+        <f>VLOOKUP($A28,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.43</v>
+      </c>
+      <c r="F28">
+        <f>VLOOKUP($A28,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>VLOOKUP($A28,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f>VLOOKUP($A28,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>VLOOKUP($A28,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="9">
+        <v>412000</v>
+      </c>
+      <c r="C29" s="11">
+        <f>VLOOKUP(A29,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>7423</v>
+      </c>
+      <c r="D29">
+        <f>VLOOKUP($A29,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>4.5</v>
+      </c>
+      <c r="E29">
+        <f>VLOOKUP($A29,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.43</v>
+      </c>
+      <c r="F29">
+        <f>VLOOKUP($A29,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f>VLOOKUP($A29,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f>VLOOKUP($A29,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f>VLOOKUP($A29,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="11">
+        <f>VLOOKUP(A30,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>8815.1</v>
+      </c>
+      <c r="D30">
+        <f>VLOOKUP($A30,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>3.5</v>
+      </c>
+      <c r="E30">
+        <f>VLOOKUP($A30,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.43</v>
+      </c>
+      <c r="F30">
+        <f>VLOOKUP($A30,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f>VLOOKUP($A30,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f>VLOOKUP($A30,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f>VLOOKUP($A30,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="6">
+        <f>ROUND(2685000*1.002*1.016*1.018*1.014*1.007,0)+600000</f>
+        <v>3441325</v>
+      </c>
+      <c r="C31" s="11">
+        <f>VLOOKUP(A31,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>24222</v>
+      </c>
+      <c r="D31">
+        <f>VLOOKUP($A31,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f>VLOOKUP($A31,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f>VLOOKUP($A31,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0.89</v>
+      </c>
+      <c r="G31">
+        <f>VLOOKUP($A31,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <f>VLOOKUP($A31,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0.89</v>
+      </c>
+      <c r="I31">
+        <f>VLOOKUP($A31,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="6">
+        <v>400000</v>
+      </c>
+      <c r="C32" s="11">
+        <f>VLOOKUP(A32,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>28000.000000000004</v>
+      </c>
+      <c r="D32">
+        <f>VLOOKUP($A32,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f>VLOOKUP($A32,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.74</v>
+      </c>
+      <c r="F32">
+        <f>VLOOKUP($A32,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f>VLOOKUP($A32,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f>VLOOKUP($A32,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f>VLOOKUP($A32,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11">
+        <f>VLOOKUP(A33,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>1700</v>
+      </c>
+      <c r="D33">
+        <f>VLOOKUP($A33,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f>VLOOKUP($A33,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>1.04</v>
+      </c>
+      <c r="F33">
+        <f>VLOOKUP($A33,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f>VLOOKUP($A33,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <f>VLOOKUP($A33,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <f>VLOOKUP($A33,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="7">
+        <v>850698.174</v>
+      </c>
+      <c r="C34" s="11">
+        <f>VLOOKUP(A34,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>27647.69067</v>
+      </c>
+      <c r="D34">
+        <f>VLOOKUP($A34,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E34">
+        <f>VLOOKUP($A34,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.6</v>
+      </c>
+      <c r="F34">
+        <f>VLOOKUP($A34,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f>VLOOKUP($A34,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f>VLOOKUP($A34,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f>VLOOKUP($A34,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="11">
+        <f>VLOOKUP(A35,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>32000</v>
+      </c>
+      <c r="D35">
+        <f>VLOOKUP($A35,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <f>VLOOKUP($A35,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.43</v>
+      </c>
+      <c r="F35">
+        <f>VLOOKUP($A35,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f>VLOOKUP($A35,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f>VLOOKUP($A35,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f>VLOOKUP($A35,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="11">
+        <f>VLOOKUP(A36,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>61528.160000000003</v>
+      </c>
+      <c r="D36">
+        <f>VLOOKUP($A36,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>3.5</v>
+      </c>
+      <c r="E36">
+        <f>VLOOKUP($A36,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.43</v>
+      </c>
+      <c r="F36">
+        <f>VLOOKUP($A36,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f>VLOOKUP($A36,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <f>VLOOKUP($A36,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f>VLOOKUP($A36,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="7">
+        <f>ROUND(2685000*1.002*1.016*1.018*1.014*1.007,0)</f>
+        <v>2841325</v>
+      </c>
+      <c r="C37" s="11">
+        <f>VLOOKUP(A37,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>14207</v>
+      </c>
+      <c r="D37">
+        <f>VLOOKUP($A37,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <f>VLOOKUP($A37,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <f>VLOOKUP($A37,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <f>VLOOKUP($A37,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <f>VLOOKUP($A37,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f>VLOOKUP($A37,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" s="9">
+        <v>730000</v>
+      </c>
+      <c r="C38" s="11">
+        <f>VLOOKUP(A38,[1]fixedCosts!$A$1:$B$23,2,0)</f>
+        <v>30000</v>
+      </c>
+      <c r="D38">
+        <f>VLOOKUP($A38,[1]techspecs!$A$1:$G$23,2,0)</f>
+        <v>2.7</v>
+      </c>
+      <c r="E38">
+        <f>VLOOKUP($A38,[1]techspecs!$A$1:$G$23,3,0)</f>
+        <v>0.85</v>
+      </c>
+      <c r="F38">
+        <f>VLOOKUP($A38,[1]techspecs!$A$1:$G$23,4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <f>VLOOKUP($A38,[1]techspecs!$A$1:$G$23,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f>VLOOKUP($A38,[1]techspecs!$A$1:$G$23,6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f>VLOOKUP($A38,[1]techspecs!$A$1:$G$23,7,0)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="13">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" s="20">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B43" s="20">
+        <v>50.29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" s="20">
+        <v>45.07</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" s="20">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="23">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="24">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" s="24">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B54" s="23">
+        <v>410</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adapting workflow to percentage load changing and load increasing by excel
</commit_message>
<xml_diff>
--- a/data/AMIRIS-EMLABpy Data inventoryREADME.xlsx
+++ b/data/AMIRIS-EMLABpy Data inventoryREADME.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C9842C-CD9B-4062-98D0-FA5281244D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81BCE2B-82EC-4BCF-88E4-5B6DE413824F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21810" yWindow="17250" windowWidth="29040" windowHeight="17640" tabRatio="858" activeTab="6" xr2:uid="{06D6063F-292D-4EBB-8494-695710908624}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="858" activeTab="6" xr2:uid="{06D6063F-292D-4EBB-8494-695710908624}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="196">
   <si>
     <t>candidate power plants</t>
   </si>
@@ -633,6 +633,9 @@
   </si>
   <si>
     <t>Equity interest rate</t>
+  </si>
+  <si>
+    <t>Initial capacity from COMPETES</t>
   </si>
 </sst>
 </file>
@@ -716,7 +719,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -752,6 +755,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -760,7 +774,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -818,6 +832,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3847,7 +3864,7 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3861,6 +3878,7 @@
     <col min="8" max="8" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3892,6 +3910,9 @@
       <c r="J1" s="26" t="s">
         <v>183</v>
       </c>
+      <c r="K1" s="34" t="s">
+        <v>195</v>
+      </c>
       <c r="Q1" s="28"/>
       <c r="R1" s="26" t="s">
         <v>104</v>

</xml_diff>